<commit_message>
search post get post comments
</commit_message>
<xml_diff>
--- a/app/src/ToDo.xlsx
+++ b/app/src/ToDo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="143">
   <si>
     <t>ActivityLogin</t>
   </si>
@@ -477,6 +477,15 @@
   <si>
     <t>post can't be liked by post's owner. Check owner of post نیازمند داشتن یوزر آیدی شخص قرار دهنده ی پست هستیم
 if post liked by user, the user shouldn't be able to like it again. Check post.isLiked این مسأله در سمت وب سرویس قبل از ثبت لایک بررسی میگردد</t>
+  </si>
+  <si>
+    <t>FragmentSearchResult</t>
+  </si>
+  <si>
+    <t>lazy load implementation</t>
+  </si>
+  <si>
+    <t>list scroll: FORCE CLOSE</t>
   </si>
 </sst>
 </file>
@@ -896,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1590,10 +1599,21 @@
       <c r="B83" s="9"/>
     </row>
     <row r="84" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="9"/>
-      <c r="B84" s="9"/>
-    </row>
-    <row r="85" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="A84" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
     <row r="86" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="87" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="88" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>